<commit_message>
Clean task 3,6,7: 4/8/2024
</commit_message>
<xml_diff>
--- a/data/BoomBust_DatafromTables.xlsx
+++ b/data/BoomBust_DatafromTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4f5e485ed766aa2/Pictures/Documents/Journal Publications/Manuscripts/Dissertation/boom-bust/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1489" documentId="8_{70A43E18-57AA-40B9-A6AA-B8B1D80A3999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{161B0ACB-3549-4428-842D-DF04F882C4F3}"/>
+  <xr:revisionPtr revIDLastSave="1490" documentId="8_{70A43E18-57AA-40B9-A6AA-B8B1D80A3999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EDEE2D8-F7C6-4F5A-B17A-9F36530C6280}"/>
   <bookViews>
-    <workbookView xWindow="1584" yWindow="1896" windowWidth="17304" windowHeight="8892" xr2:uid="{8025EA18-20DD-4AB1-8E18-97042F4F59FB}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8025EA18-20DD-4AB1-8E18-97042F4F59FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -242,9 +242,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>mon-Year</t>
-  </si>
-  <si>
     <t>Density (n/m^2)</t>
   </si>
   <si>
@@ -258,6 +255,9 @@
   </si>
   <si>
     <t>Density (n/0.25m^2)</t>
+  </si>
+  <si>
+    <t>Mon-Year</t>
   </si>
 </sst>
 </file>
@@ -650,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A607EED-BDE6-4E7B-8223-CBB56B106F2E}">
   <dimension ref="A1:H469"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G319" sqref="G319"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2309,10 +2309,10 @@
         <v>9</v>
       </c>
       <c r="G78" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H78" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
@@ -2335,10 +2335,10 @@
         <v>8</v>
       </c>
       <c r="G79" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H79" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
@@ -2361,10 +2361,10 @@
         <v>6</v>
       </c>
       <c r="G80" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H80" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
@@ -2387,10 +2387,10 @@
         <v>8</v>
       </c>
       <c r="G81" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H81" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
@@ -2413,10 +2413,10 @@
         <v>5</v>
       </c>
       <c r="G82" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H82" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
@@ -2439,10 +2439,10 @@
         <v>9</v>
       </c>
       <c r="G83" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H83" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
@@ -2465,10 +2465,10 @@
         <v>6</v>
       </c>
       <c r="G84" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H84" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
@@ -2491,10 +2491,10 @@
         <v>8</v>
       </c>
       <c r="G85" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H85" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
@@ -2517,10 +2517,10 @@
         <v>9</v>
       </c>
       <c r="G86" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H86" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
@@ -2543,10 +2543,10 @@
         <v>8</v>
       </c>
       <c r="G87" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H87" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
@@ -2569,10 +2569,10 @@
         <v>10</v>
       </c>
       <c r="G88" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H88" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
@@ -2595,10 +2595,10 @@
         <v>6</v>
       </c>
       <c r="G89" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H89" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
@@ -2621,10 +2621,10 @@
         <v>8</v>
       </c>
       <c r="G90" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H90" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
@@ -2647,10 +2647,10 @@
         <v>5</v>
       </c>
       <c r="G91" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H91" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
@@ -2673,10 +2673,10 @@
         <v>9</v>
       </c>
       <c r="G92" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H92" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
@@ -2699,10 +2699,10 @@
         <v>6</v>
       </c>
       <c r="G93" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H93" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
@@ -2725,10 +2725,10 @@
         <v>8</v>
       </c>
       <c r="G94" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H94" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
@@ -2749,7 +2749,7 @@
         <v>2007</v>
       </c>
       <c r="G95" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H95" t="s">
         <v>67</v>
@@ -2773,7 +2773,7 @@
         <v>2012</v>
       </c>
       <c r="G96" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H96" t="s">
         <v>67</v>
@@ -2797,7 +2797,7 @@
         <v>2013</v>
       </c>
       <c r="G97" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H97" t="s">
         <v>67</v>
@@ -2821,7 +2821,7 @@
         <v>2014</v>
       </c>
       <c r="G98" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H98" t="s">
         <v>67</v>
@@ -2844,7 +2844,7 @@
         <v>1995</v>
       </c>
       <c r="G99" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H99" t="s">
         <v>67</v>
@@ -2867,7 +2867,7 @@
         <v>1999</v>
       </c>
       <c r="G100" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H100" t="s">
         <v>67</v>
@@ -2890,7 +2890,7 @@
         <v>2003</v>
       </c>
       <c r="G101" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H101" t="s">
         <v>67</v>
@@ -2913,7 +2913,7 @@
         <v>1995</v>
       </c>
       <c r="G102" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H102" t="s">
         <v>67</v>
@@ -2936,7 +2936,7 @@
         <v>1999</v>
       </c>
       <c r="G103" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H103" t="s">
         <v>67</v>
@@ -2959,7 +2959,7 @@
         <v>2003</v>
       </c>
       <c r="G104" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H104" t="s">
         <v>67</v>
@@ -2982,7 +2982,7 @@
         <v>1995</v>
       </c>
       <c r="G105" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H105" t="s">
         <v>67</v>
@@ -3005,7 +3005,7 @@
         <v>1999</v>
       </c>
       <c r="G106" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H106" t="s">
         <v>67</v>
@@ -3028,7 +3028,7 @@
         <v>2003</v>
       </c>
       <c r="G107" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H107" t="s">
         <v>67</v>
@@ -3048,7 +3048,7 @@
         <v>1958</v>
       </c>
       <c r="G108" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H108" t="s">
         <v>67</v>
@@ -3068,7 +3068,7 @@
         <v>1963</v>
       </c>
       <c r="G109" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H109" t="s">
         <v>67</v>
@@ -3088,7 +3088,7 @@
         <v>1964</v>
       </c>
       <c r="G110" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H110" t="s">
         <v>67</v>
@@ -3108,7 +3108,7 @@
         <v>1965</v>
       </c>
       <c r="G111" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H111" t="s">
         <v>67</v>
@@ -3128,7 +3128,7 @@
         <v>1966</v>
       </c>
       <c r="G112" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H112" t="s">
         <v>67</v>
@@ -3148,7 +3148,7 @@
         <v>1967</v>
       </c>
       <c r="G113" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H113" t="s">
         <v>67</v>
@@ -3168,7 +3168,7 @@
         <v>1969</v>
       </c>
       <c r="G114" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H114" t="s">
         <v>67</v>
@@ -3188,7 +3188,7 @@
         <v>1975</v>
       </c>
       <c r="G115" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H115" t="s">
         <v>67</v>
@@ -3208,7 +3208,7 @@
         <v>1979</v>
       </c>
       <c r="G116" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H116" t="s">
         <v>67</v>
@@ -3228,7 +3228,7 @@
         <v>1980</v>
       </c>
       <c r="G117" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H117" t="s">
         <v>67</v>
@@ -3248,7 +3248,7 @@
         <v>1982</v>
       </c>
       <c r="G118" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H118" t="s">
         <v>67</v>
@@ -3268,7 +3268,7 @@
         <v>1983</v>
       </c>
       <c r="G119" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H119" t="s">
         <v>67</v>
@@ -3288,7 +3288,7 @@
         <v>1999</v>
       </c>
       <c r="G120" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H120" t="s">
         <v>67</v>
@@ -3308,7 +3308,7 @@
         <v>2000</v>
       </c>
       <c r="G121" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H121" t="s">
         <v>67</v>
@@ -3328,7 +3328,7 @@
         <v>2002</v>
       </c>
       <c r="G122" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H122" t="s">
         <v>67</v>
@@ -3348,7 +3348,7 @@
         <v>2003</v>
       </c>
       <c r="G123" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H123" t="s">
         <v>67</v>
@@ -3368,7 +3368,7 @@
         <v>2004</v>
       </c>
       <c r="G124" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H124" t="s">
         <v>67</v>
@@ -3388,7 +3388,7 @@
         <v>1958</v>
       </c>
       <c r="G125" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H125" t="s">
         <v>67</v>
@@ -3408,7 +3408,7 @@
         <v>1963</v>
       </c>
       <c r="G126" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H126" t="s">
         <v>67</v>
@@ -3428,7 +3428,7 @@
         <v>1964</v>
       </c>
       <c r="G127" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H127" t="s">
         <v>67</v>
@@ -3448,7 +3448,7 @@
         <v>1965</v>
       </c>
       <c r="G128" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H128" t="s">
         <v>67</v>
@@ -3468,7 +3468,7 @@
         <v>1966</v>
       </c>
       <c r="G129" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H129" t="s">
         <v>67</v>
@@ -3488,7 +3488,7 @@
         <v>1967</v>
       </c>
       <c r="G130" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H130" t="s">
         <v>67</v>
@@ -3508,7 +3508,7 @@
         <v>1969</v>
       </c>
       <c r="G131" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H131" t="s">
         <v>67</v>
@@ -3528,7 +3528,7 @@
         <v>1975</v>
       </c>
       <c r="G132" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H132" t="s">
         <v>67</v>
@@ -3548,7 +3548,7 @@
         <v>1979</v>
       </c>
       <c r="G133" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H133" t="s">
         <v>67</v>
@@ -3568,7 +3568,7 @@
         <v>1980</v>
       </c>
       <c r="G134" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H134" t="s">
         <v>67</v>
@@ -3588,7 +3588,7 @@
         <v>1982</v>
       </c>
       <c r="G135" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H135" t="s">
         <v>67</v>
@@ -3608,7 +3608,7 @@
         <v>1983</v>
       </c>
       <c r="G136" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H136" t="s">
         <v>67</v>
@@ -3628,7 +3628,7 @@
         <v>1999</v>
       </c>
       <c r="G137" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H137" t="s">
         <v>67</v>
@@ -3648,7 +3648,7 @@
         <v>2000</v>
       </c>
       <c r="G138" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H138" t="s">
         <v>67</v>
@@ -3668,7 +3668,7 @@
         <v>2002</v>
       </c>
       <c r="G139" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H139" t="s">
         <v>67</v>
@@ -3688,7 +3688,7 @@
         <v>2003</v>
       </c>
       <c r="G140" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H140" t="s">
         <v>67</v>
@@ -3708,7 +3708,7 @@
         <v>2004</v>
       </c>
       <c r="G141" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H141" t="s">
         <v>67</v>
@@ -3728,7 +3728,7 @@
         <v>1958</v>
       </c>
       <c r="G142" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H142" t="s">
         <v>67</v>
@@ -3748,7 +3748,7 @@
         <v>1963</v>
       </c>
       <c r="G143" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H143" t="s">
         <v>67</v>
@@ -3768,7 +3768,7 @@
         <v>1964</v>
       </c>
       <c r="G144" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H144" t="s">
         <v>67</v>
@@ -3788,7 +3788,7 @@
         <v>1965</v>
       </c>
       <c r="G145" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H145" t="s">
         <v>67</v>
@@ -3808,7 +3808,7 @@
         <v>1966</v>
       </c>
       <c r="G146" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H146" t="s">
         <v>67</v>
@@ -3828,7 +3828,7 @@
         <v>1967</v>
       </c>
       <c r="G147" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H147" t="s">
         <v>67</v>
@@ -3848,7 +3848,7 @@
         <v>1969</v>
       </c>
       <c r="G148" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H148" t="s">
         <v>67</v>
@@ -3868,7 +3868,7 @@
         <v>1975</v>
       </c>
       <c r="G149" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H149" t="s">
         <v>67</v>
@@ -3888,7 +3888,7 @@
         <v>1979</v>
       </c>
       <c r="G150" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H150" t="s">
         <v>67</v>
@@ -3908,7 +3908,7 @@
         <v>1980</v>
       </c>
       <c r="G151" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H151" t="s">
         <v>67</v>
@@ -3928,7 +3928,7 @@
         <v>1982</v>
       </c>
       <c r="G152" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H152" t="s">
         <v>67</v>
@@ -3948,7 +3948,7 @@
         <v>1983</v>
       </c>
       <c r="G153" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H153" t="s">
         <v>67</v>
@@ -3968,7 +3968,7 @@
         <v>1999</v>
       </c>
       <c r="G154" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H154" t="s">
         <v>67</v>
@@ -3988,7 +3988,7 @@
         <v>2000</v>
       </c>
       <c r="G155" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H155" t="s">
         <v>67</v>
@@ -4008,7 +4008,7 @@
         <v>2002</v>
       </c>
       <c r="G156" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H156" t="s">
         <v>67</v>
@@ -4028,7 +4028,7 @@
         <v>2003</v>
       </c>
       <c r="G157" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H157" t="s">
         <v>67</v>
@@ -4048,7 +4048,7 @@
         <v>2004</v>
       </c>
       <c r="G158" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H158" t="s">
         <v>67</v>
@@ -4068,7 +4068,7 @@
         <v>1958</v>
       </c>
       <c r="G159" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H159" t="s">
         <v>67</v>
@@ -4088,7 +4088,7 @@
         <v>1963</v>
       </c>
       <c r="G160" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H160" t="s">
         <v>67</v>
@@ -4108,7 +4108,7 @@
         <v>1964</v>
       </c>
       <c r="G161" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H161" t="s">
         <v>67</v>
@@ -4128,7 +4128,7 @@
         <v>1965</v>
       </c>
       <c r="G162" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H162" t="s">
         <v>67</v>
@@ -4148,7 +4148,7 @@
         <v>1966</v>
       </c>
       <c r="G163" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H163" t="s">
         <v>67</v>
@@ -4168,7 +4168,7 @@
         <v>1967</v>
       </c>
       <c r="G164" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H164" t="s">
         <v>67</v>
@@ -4188,7 +4188,7 @@
         <v>1969</v>
       </c>
       <c r="G165" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H165" t="s">
         <v>67</v>
@@ -4208,7 +4208,7 @@
         <v>1975</v>
       </c>
       <c r="G166" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H166" t="s">
         <v>67</v>
@@ -4228,7 +4228,7 @@
         <v>1979</v>
       </c>
       <c r="G167" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H167" t="s">
         <v>67</v>
@@ -4248,7 +4248,7 @@
         <v>1980</v>
       </c>
       <c r="G168" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H168" t="s">
         <v>67</v>
@@ -4268,7 +4268,7 @@
         <v>1982</v>
       </c>
       <c r="G169" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H169" t="s">
         <v>67</v>
@@ -4288,7 +4288,7 @@
         <v>1983</v>
       </c>
       <c r="G170" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H170" t="s">
         <v>67</v>
@@ -4308,7 +4308,7 @@
         <v>1999</v>
       </c>
       <c r="G171" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H171" t="s">
         <v>67</v>
@@ -4328,7 +4328,7 @@
         <v>2000</v>
       </c>
       <c r="G172" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H172" t="s">
         <v>67</v>
@@ -4348,7 +4348,7 @@
         <v>2002</v>
       </c>
       <c r="G173" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H173" t="s">
         <v>67</v>
@@ -4368,7 +4368,7 @@
         <v>2003</v>
       </c>
       <c r="G174" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H174" t="s">
         <v>67</v>
@@ -4388,7 +4388,7 @@
         <v>2004</v>
       </c>
       <c r="G175" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H175" t="s">
         <v>67</v>
@@ -4414,10 +4414,10 @@
         <v>5</v>
       </c>
       <c r="G176" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H176" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.3">
@@ -4440,10 +4440,10 @@
         <v>8</v>
       </c>
       <c r="G177" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H177" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.3">
@@ -4466,10 +4466,10 @@
         <v>6</v>
       </c>
       <c r="G178" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H178" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.3">
@@ -4492,10 +4492,10 @@
         <v>9</v>
       </c>
       <c r="G179" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H179" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.3">
@@ -4518,10 +4518,10 @@
         <v>7</v>
       </c>
       <c r="G180" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H180" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.3">
@@ -4544,10 +4544,10 @@
         <v>4</v>
       </c>
       <c r="G181" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H181" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.3">
@@ -4570,10 +4570,10 @@
         <v>8</v>
       </c>
       <c r="G182" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H182" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.3">
@@ -4596,10 +4596,10 @@
         <v>5</v>
       </c>
       <c r="G183" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H183" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.3">
@@ -4622,10 +4622,10 @@
         <v>8</v>
       </c>
       <c r="G184" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H184" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.3">
@@ -4648,10 +4648,10 @@
         <v>5</v>
       </c>
       <c r="G185" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H185" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.3">
@@ -4674,10 +4674,10 @@
         <v>8</v>
       </c>
       <c r="G186" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H186" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.3">
@@ -4700,10 +4700,10 @@
         <v>7</v>
       </c>
       <c r="G187" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H187" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.3">
@@ -4726,10 +4726,10 @@
         <v>4</v>
       </c>
       <c r="G188" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H188" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.3">
@@ -4752,10 +4752,10 @@
         <v>8</v>
       </c>
       <c r="G189" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H189" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.3">
@@ -4778,10 +4778,10 @@
         <v>5</v>
       </c>
       <c r="G190" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H190" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.3">
@@ -4804,10 +4804,10 @@
         <v>8</v>
       </c>
       <c r="G191" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H191" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.3">
@@ -4830,10 +4830,10 @@
         <v>7</v>
       </c>
       <c r="G192" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H192" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.3">
@@ -4856,10 +4856,10 @@
         <v>9</v>
       </c>
       <c r="G193" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H193" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.3">
@@ -4882,10 +4882,10 @@
         <v>7</v>
       </c>
       <c r="G194" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H194" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.3">
@@ -4908,10 +4908,10 @@
         <v>4</v>
       </c>
       <c r="G195" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H195" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.3">
@@ -4934,10 +4934,10 @@
         <v>8</v>
       </c>
       <c r="G196" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H196" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.3">
@@ -4960,10 +4960,10 @@
         <v>4</v>
       </c>
       <c r="G197" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H197" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.3">
@@ -4986,10 +4986,10 @@
         <v>9</v>
       </c>
       <c r="G198" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H198" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.3">
@@ -5012,10 +5012,10 @@
         <v>6</v>
       </c>
       <c r="G199" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H199" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.3">
@@ -5038,10 +5038,10 @@
         <v>9</v>
       </c>
       <c r="G200" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H200" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.3">
@@ -5064,10 +5064,10 @@
         <v>7</v>
       </c>
       <c r="G201" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H201" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.3">
@@ -5090,10 +5090,10 @@
         <v>4</v>
       </c>
       <c r="G202" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H202" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.3">
@@ -5116,10 +5116,10 @@
         <v>8</v>
       </c>
       <c r="G203" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H203" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.3">
@@ -5142,10 +5142,10 @@
         <v>5</v>
       </c>
       <c r="G204" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H204" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.3">
@@ -5168,10 +5168,10 @@
         <v>9</v>
       </c>
       <c r="G205" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H205" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.3">
@@ -5194,10 +5194,10 @@
         <v>5</v>
       </c>
       <c r="G206" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H206" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.3">
@@ -5220,10 +5220,10 @@
         <v>9</v>
       </c>
       <c r="G207" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H207" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.3">
@@ -5246,10 +5246,10 @@
         <v>8</v>
       </c>
       <c r="G208" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H208" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.3">
@@ -5272,10 +5272,10 @@
         <v>3</v>
       </c>
       <c r="G209" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H209" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.3">
@@ -5298,10 +5298,10 @@
         <v>7</v>
       </c>
       <c r="G210" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H210" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.3">
@@ -5324,10 +5324,10 @@
         <v>5</v>
       </c>
       <c r="G211" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H211" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.3">
@@ -5350,10 +5350,10 @@
         <v>8</v>
       </c>
       <c r="G212" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H212" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.3">
@@ -5376,10 +5376,10 @@
         <v>6</v>
       </c>
       <c r="G213" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H213" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.3">
@@ -5402,10 +5402,10 @@
         <v>9</v>
       </c>
       <c r="G214" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H214" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.3">
@@ -5428,10 +5428,10 @@
         <v>8</v>
       </c>
       <c r="G215" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H215" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.3">
@@ -5454,10 +5454,10 @@
         <v>3</v>
       </c>
       <c r="G216" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H216" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.3">
@@ -5480,10 +5480,10 @@
         <v>7</v>
       </c>
       <c r="G217" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H217" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.3">
@@ -5506,10 +5506,10 @@
         <v>5</v>
       </c>
       <c r="G218" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H218" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.3">
@@ -5532,10 +5532,10 @@
         <v>9</v>
       </c>
       <c r="G219" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H219" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.3">
@@ -5558,10 +5558,10 @@
         <v>6</v>
       </c>
       <c r="G220" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H220" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.3">
@@ -5584,10 +5584,10 @@
         <v>10</v>
       </c>
       <c r="G221" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H221" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.3">
@@ -5610,10 +5610,10 @@
         <v>8</v>
       </c>
       <c r="G222" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H222" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.3">
@@ -5636,10 +5636,10 @@
         <v>2</v>
       </c>
       <c r="G223" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H223" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.3">
@@ -5662,10 +5662,10 @@
         <v>7</v>
       </c>
       <c r="G224" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H224" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.3">
@@ -5688,10 +5688,10 @@
         <v>6</v>
       </c>
       <c r="G225" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H225" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.3">
@@ -5714,10 +5714,10 @@
         <v>9</v>
       </c>
       <c r="G226" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H226" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.3">
@@ -5740,10 +5740,10 @@
         <v>6</v>
       </c>
       <c r="G227" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H227" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.3">
@@ -5766,10 +5766,10 @@
         <v>9</v>
       </c>
       <c r="G228" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H228" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.3">
@@ -5792,10 +5792,10 @@
         <v>8</v>
       </c>
       <c r="G229" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H229" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.3">
@@ -5818,10 +5818,10 @@
         <v>2</v>
       </c>
       <c r="G230" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H230" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.3">
@@ -5844,10 +5844,10 @@
         <v>7</v>
       </c>
       <c r="G231" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H231" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.3">
@@ -5870,10 +5870,10 @@
         <v>6</v>
       </c>
       <c r="G232" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H232" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.3">
@@ -5896,10 +5896,10 @@
         <v>9</v>
       </c>
       <c r="G233" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H233" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.3">
@@ -5922,10 +5922,10 @@
         <v>6</v>
       </c>
       <c r="G234" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H234" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.3">
@@ -5948,10 +5948,10 @@
         <v>9</v>
       </c>
       <c r="G235" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H235" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.3">
@@ -5974,10 +5974,10 @@
         <v>9</v>
       </c>
       <c r="G236" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H236" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.3">
@@ -6000,10 +6000,10 @@
         <v>2</v>
       </c>
       <c r="G237" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H237" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.3">
@@ -6026,10 +6026,10 @@
         <v>8</v>
       </c>
       <c r="G238" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H238" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.3">
@@ -6052,10 +6052,10 @@
         <v>5</v>
       </c>
       <c r="G239" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H239" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.3">
@@ -6078,10 +6078,10 @@
         <v>9</v>
       </c>
       <c r="G240" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H240" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.3">
@@ -6104,10 +6104,10 @@
         <v>6</v>
       </c>
       <c r="G241" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H241" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.3">
@@ -6130,10 +6130,10 @@
         <v>9</v>
       </c>
       <c r="G242" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H242" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.3">
@@ -6156,10 +6156,10 @@
         <v>8</v>
       </c>
       <c r="G243" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H243" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.3">
@@ -6182,10 +6182,10 @@
         <v>3</v>
       </c>
       <c r="G244" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H244" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.3">
@@ -6208,10 +6208,10 @@
         <v>8</v>
       </c>
       <c r="G245" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H245" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.3">
@@ -7910,7 +7910,7 @@
         <v>2011</v>
       </c>
       <c r="G319" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H319" t="s">
         <v>67</v>
@@ -7933,7 +7933,7 @@
         <v>2015</v>
       </c>
       <c r="G320" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H320" t="s">
         <v>67</v>
@@ -7956,7 +7956,7 @@
         <v>2018</v>
       </c>
       <c r="G321" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H321" t="s">
         <v>67</v>
@@ -7979,7 +7979,7 @@
         <v>2011</v>
       </c>
       <c r="G322" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H322" t="s">
         <v>67</v>
@@ -8002,7 +8002,7 @@
         <v>2015</v>
       </c>
       <c r="G323" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H323" t="s">
         <v>67</v>
@@ -8025,7 +8025,7 @@
         <v>2017</v>
       </c>
       <c r="G324" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H324" t="s">
         <v>67</v>
@@ -8048,7 +8048,7 @@
         <v>2018</v>
       </c>
       <c r="G325" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H325" t="s">
         <v>67</v>
@@ -8071,7 +8071,7 @@
         <v>2011</v>
       </c>
       <c r="G326" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H326" t="s">
         <v>67</v>
@@ -8094,7 +8094,7 @@
         <v>2015</v>
       </c>
       <c r="G327" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H327" t="s">
         <v>67</v>
@@ -8117,7 +8117,7 @@
         <v>2017</v>
       </c>
       <c r="G328" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H328" t="s">
         <v>67</v>
@@ -8140,7 +8140,7 @@
         <v>2018</v>
       </c>
       <c r="G329" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H329" t="s">
         <v>67</v>
@@ -8163,7 +8163,7 @@
         <v>1997</v>
       </c>
       <c r="G330" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H330" t="s">
         <v>67</v>
@@ -8186,7 +8186,7 @@
         <v>2015</v>
       </c>
       <c r="G331" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H331" t="s">
         <v>67</v>
@@ -8209,7 +8209,7 @@
         <v>2016</v>
       </c>
       <c r="G332" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H332" t="s">
         <v>67</v>
@@ -8232,7 +8232,7 @@
         <v>2017</v>
       </c>
       <c r="G333" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H333" t="s">
         <v>67</v>
@@ -8255,7 +8255,7 @@
         <v>2018</v>
       </c>
       <c r="G334" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H334" t="s">
         <v>67</v>
@@ -8278,7 +8278,7 @@
         <v>1997</v>
       </c>
       <c r="G335" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H335" t="s">
         <v>67</v>
@@ -8301,7 +8301,7 @@
         <v>2015</v>
       </c>
       <c r="G336" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H336" t="s">
         <v>67</v>
@@ -8324,7 +8324,7 @@
         <v>2016</v>
       </c>
       <c r="G337" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H337" t="s">
         <v>67</v>
@@ -8347,7 +8347,7 @@
         <v>2017</v>
       </c>
       <c r="G338" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H338" t="s">
         <v>67</v>
@@ -8370,7 +8370,7 @@
         <v>2018</v>
       </c>
       <c r="G339" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H339" t="s">
         <v>67</v>
@@ -8393,7 +8393,7 @@
         <v>2011</v>
       </c>
       <c r="G340" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H340" t="s">
         <v>67</v>
@@ -8416,7 +8416,7 @@
         <v>2015</v>
       </c>
       <c r="G341" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H341" t="s">
         <v>67</v>
@@ -8439,7 +8439,7 @@
         <v>2016</v>
       </c>
       <c r="G342" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H342" t="s">
         <v>67</v>
@@ -8462,7 +8462,7 @@
         <v>2017</v>
       </c>
       <c r="G343" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H343" t="s">
         <v>67</v>
@@ -8485,7 +8485,7 @@
         <v>2018</v>
       </c>
       <c r="G344" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H344" t="s">
         <v>67</v>
@@ -8508,7 +8508,7 @@
         <v>2011</v>
       </c>
       <c r="G345" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H345" t="s">
         <v>67</v>
@@ -8531,7 +8531,7 @@
         <v>2015</v>
       </c>
       <c r="G346" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H346" t="s">
         <v>67</v>
@@ -8554,7 +8554,7 @@
         <v>2017</v>
       </c>
       <c r="G347" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H347" t="s">
         <v>67</v>
@@ -8577,7 +8577,7 @@
         <v>2018</v>
       </c>
       <c r="G348" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H348" t="s">
         <v>67</v>
@@ -8600,7 +8600,7 @@
         <v>2015</v>
       </c>
       <c r="G349" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H349" t="s">
         <v>67</v>
@@ -8623,7 +8623,7 @@
         <v>2017</v>
       </c>
       <c r="G350" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H350" t="s">
         <v>67</v>
@@ -8646,7 +8646,7 @@
         <v>2018</v>
       </c>
       <c r="G351" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H351" t="s">
         <v>67</v>
@@ -8666,7 +8666,7 @@
         <v>1963</v>
       </c>
       <c r="G352" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H352" t="s">
         <v>67</v>
@@ -8686,7 +8686,7 @@
         <v>1966</v>
       </c>
       <c r="G353" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H353" t="s">
         <v>67</v>
@@ -8706,7 +8706,7 @@
         <v>1969</v>
       </c>
       <c r="G354" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H354" t="s">
         <v>67</v>
@@ -8726,7 +8726,7 @@
         <v>1976</v>
       </c>
       <c r="G355" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H355" t="s">
         <v>67</v>
@@ -8746,7 +8746,7 @@
         <v>1977</v>
       </c>
       <c r="G356" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H356" t="s">
         <v>67</v>
@@ -8766,7 +8766,7 @@
         <v>1978</v>
       </c>
       <c r="G357" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H357" t="s">
         <v>67</v>
@@ -8786,7 +8786,7 @@
         <v>1979</v>
       </c>
       <c r="G358" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H358" t="s">
         <v>67</v>
@@ -8806,7 +8806,7 @@
         <v>1980</v>
       </c>
       <c r="G359" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H359" t="s">
         <v>67</v>
@@ -8826,7 +8826,7 @@
         <v>1981</v>
       </c>
       <c r="G360" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H360" t="s">
         <v>67</v>
@@ -8846,7 +8846,7 @@
         <v>1982</v>
       </c>
       <c r="G361" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H361" t="s">
         <v>67</v>
@@ -8866,7 +8866,7 @@
         <v>1983</v>
       </c>
       <c r="G362" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H362" t="s">
         <v>67</v>
@@ -8886,7 +8886,7 @@
         <v>1984</v>
       </c>
       <c r="G363" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H363" t="s">
         <v>67</v>
@@ -8906,7 +8906,7 @@
         <v>1985</v>
       </c>
       <c r="G364" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H364" t="s">
         <v>67</v>
@@ -8926,7 +8926,7 @@
         <v>1986</v>
       </c>
       <c r="G365" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H365" t="s">
         <v>67</v>
@@ -8946,7 +8946,7 @@
         <v>1987</v>
       </c>
       <c r="G366" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H366" t="s">
         <v>67</v>
@@ -8966,7 +8966,7 @@
         <v>1988</v>
       </c>
       <c r="G367" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H367" t="s">
         <v>67</v>
@@ -8986,7 +8986,7 @@
         <v>1989</v>
       </c>
       <c r="G368" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H368" t="s">
         <v>67</v>
@@ -9006,7 +9006,7 @@
         <v>1990</v>
       </c>
       <c r="G369" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H369" t="s">
         <v>67</v>
@@ -9026,7 +9026,7 @@
         <v>1995</v>
       </c>
       <c r="G370" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H370" t="s">
         <v>67</v>
@@ -9046,7 +9046,7 @@
         <v>2001</v>
       </c>
       <c r="G371" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H371" t="s">
         <v>67</v>
@@ -9066,7 +9066,7 @@
         <v>2002</v>
       </c>
       <c r="G372" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H372" t="s">
         <v>67</v>
@@ -9086,7 +9086,7 @@
         <v>2003</v>
       </c>
       <c r="G373" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H373" t="s">
         <v>67</v>
@@ -9106,7 +9106,7 @@
         <v>2004</v>
       </c>
       <c r="G374" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H374" t="s">
         <v>67</v>
@@ -9126,7 +9126,7 @@
         <v>2005</v>
       </c>
       <c r="G375" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H375" t="s">
         <v>67</v>
@@ -9146,7 +9146,7 @@
         <v>2006</v>
       </c>
       <c r="G376" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H376" t="s">
         <v>67</v>
@@ -9166,7 +9166,7 @@
         <v>2007</v>
       </c>
       <c r="G377" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H377" t="s">
         <v>67</v>
@@ -9186,7 +9186,7 @@
         <v>2001</v>
       </c>
       <c r="G378" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H378" t="s">
         <v>67</v>
@@ -9206,7 +9206,7 @@
         <v>2002</v>
       </c>
       <c r="G379" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H379" t="s">
         <v>67</v>
@@ -9226,7 +9226,7 @@
         <v>2003</v>
       </c>
       <c r="G380" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H380" t="s">
         <v>67</v>
@@ -9246,7 +9246,7 @@
         <v>2004</v>
       </c>
       <c r="G381" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H381" t="s">
         <v>67</v>
@@ -9266,7 +9266,7 @@
         <v>2005</v>
       </c>
       <c r="G382" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H382" t="s">
         <v>67</v>
@@ -9286,7 +9286,7 @@
         <v>2006</v>
       </c>
       <c r="G383" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H383" t="s">
         <v>67</v>
@@ -9306,7 +9306,7 @@
         <v>2007</v>
       </c>
       <c r="G384" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H384" t="s">
         <v>67</v>
@@ -9326,7 +9326,7 @@
         <v>2008</v>
       </c>
       <c r="G385" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H385" t="s">
         <v>67</v>
@@ -9346,7 +9346,7 @@
         <v>2009</v>
       </c>
       <c r="G386" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H386" t="s">
         <v>67</v>
@@ -9366,7 +9366,7 @@
         <v>2002</v>
       </c>
       <c r="G387" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H387" t="s">
         <v>67</v>
@@ -9386,7 +9386,7 @@
         <v>2003</v>
       </c>
       <c r="G388" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H388" t="s">
         <v>67</v>
@@ -9406,7 +9406,7 @@
         <v>2004</v>
       </c>
       <c r="G389" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H389" t="s">
         <v>67</v>
@@ -9426,7 +9426,7 @@
         <v>2005</v>
       </c>
       <c r="G390" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H390" t="s">
         <v>67</v>
@@ -9446,7 +9446,7 @@
         <v>2006</v>
       </c>
       <c r="G391" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H391" t="s">
         <v>67</v>
@@ -9466,7 +9466,7 @@
         <v>2007</v>
       </c>
       <c r="G392" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H392" t="s">
         <v>67</v>
@@ -9486,7 +9486,7 @@
         <v>2008</v>
       </c>
       <c r="G393" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H393" t="s">
         <v>67</v>
@@ -9509,7 +9509,7 @@
         <v>1911</v>
       </c>
       <c r="G394" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H394" t="s">
         <v>67</v>
@@ -9532,7 +9532,7 @@
         <v>1912</v>
       </c>
       <c r="G395" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H395" t="s">
         <v>67</v>
@@ -9555,7 +9555,7 @@
         <v>1913</v>
       </c>
       <c r="G396" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H396" t="s">
         <v>67</v>
@@ -9578,7 +9578,7 @@
         <v>1914</v>
       </c>
       <c r="G397" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H397" t="s">
         <v>67</v>
@@ -9601,7 +9601,7 @@
         <v>1915</v>
       </c>
       <c r="G398" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H398" t="s">
         <v>67</v>
@@ -9624,7 +9624,7 @@
         <v>1916</v>
       </c>
       <c r="G399" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H399" t="s">
         <v>67</v>
@@ -9647,7 +9647,7 @@
         <v>1917</v>
       </c>
       <c r="G400" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H400" t="s">
         <v>67</v>
@@ -9670,7 +9670,7 @@
         <v>1918</v>
       </c>
       <c r="G401" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H401" t="s">
         <v>67</v>
@@ -9693,7 +9693,7 @@
         <v>1919</v>
       </c>
       <c r="G402" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H402" t="s">
         <v>67</v>
@@ -9716,7 +9716,7 @@
         <v>1920</v>
       </c>
       <c r="G403" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H403" t="s">
         <v>67</v>
@@ -9739,7 +9739,7 @@
         <v>1921</v>
       </c>
       <c r="G404" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H404" t="s">
         <v>67</v>
@@ -9762,7 +9762,7 @@
         <v>1922</v>
       </c>
       <c r="G405" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H405" t="s">
         <v>67</v>
@@ -9785,7 +9785,7 @@
         <v>1923</v>
       </c>
       <c r="G406" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H406" t="s">
         <v>67</v>
@@ -9808,7 +9808,7 @@
         <v>1924</v>
       </c>
       <c r="G407" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H407" t="s">
         <v>67</v>
@@ -9831,7 +9831,7 @@
         <v>1925</v>
       </c>
       <c r="G408" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H408" t="s">
         <v>67</v>
@@ -9854,7 +9854,7 @@
         <v>1926</v>
       </c>
       <c r="G409" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H409" t="s">
         <v>67</v>
@@ -9877,7 +9877,7 @@
         <v>1927</v>
       </c>
       <c r="G410" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H410" t="s">
         <v>67</v>
@@ -9900,7 +9900,7 @@
         <v>1928</v>
       </c>
       <c r="G411" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H411" t="s">
         <v>67</v>
@@ -9923,7 +9923,7 @@
         <v>1929</v>
       </c>
       <c r="G412" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H412" t="s">
         <v>67</v>
@@ -9946,7 +9946,7 @@
         <v>1930</v>
       </c>
       <c r="G413" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H413" t="s">
         <v>67</v>
@@ -9969,7 +9969,7 @@
         <v>1931</v>
       </c>
       <c r="G414" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H414" t="s">
         <v>67</v>
@@ -9992,7 +9992,7 @@
         <v>1932</v>
       </c>
       <c r="G415" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H415" t="s">
         <v>67</v>
@@ -10015,7 +10015,7 @@
         <v>1933</v>
       </c>
       <c r="G416" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H416" t="s">
         <v>67</v>
@@ -10038,7 +10038,7 @@
         <v>1934</v>
       </c>
       <c r="G417" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H417" t="s">
         <v>67</v>
@@ -10061,7 +10061,7 @@
         <v>1935</v>
       </c>
       <c r="G418" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H418" t="s">
         <v>67</v>
@@ -10084,7 +10084,7 @@
         <v>1936</v>
       </c>
       <c r="G419" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H419" t="s">
         <v>67</v>
@@ -10107,7 +10107,7 @@
         <v>1937</v>
       </c>
       <c r="G420" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H420" t="s">
         <v>67</v>
@@ -10130,7 +10130,7 @@
         <v>1938</v>
       </c>
       <c r="G421" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H421" t="s">
         <v>67</v>
@@ -10153,7 +10153,7 @@
         <v>1939</v>
       </c>
       <c r="G422" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H422" t="s">
         <v>67</v>
@@ -10176,7 +10176,7 @@
         <v>1940</v>
       </c>
       <c r="G423" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H423" t="s">
         <v>67</v>
@@ -10199,7 +10199,7 @@
         <v>1941</v>
       </c>
       <c r="G424" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H424" t="s">
         <v>67</v>
@@ -10222,7 +10222,7 @@
         <v>1946</v>
       </c>
       <c r="G425" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H425" t="s">
         <v>67</v>
@@ -10245,7 +10245,7 @@
         <v>1947</v>
       </c>
       <c r="G426" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H426" t="s">
         <v>67</v>
@@ -10268,7 +10268,7 @@
         <v>1948</v>
       </c>
       <c r="G427" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H427" t="s">
         <v>67</v>
@@ -10291,7 +10291,7 @@
         <v>1949</v>
       </c>
       <c r="G428" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H428" t="s">
         <v>67</v>
@@ -10314,7 +10314,7 @@
         <v>1950</v>
       </c>
       <c r="G429" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H429" t="s">
         <v>67</v>
@@ -10337,7 +10337,7 @@
         <v>1911</v>
       </c>
       <c r="G430" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H430" t="s">
         <v>67</v>
@@ -10360,7 +10360,7 @@
         <v>1912</v>
       </c>
       <c r="G431" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H431" t="s">
         <v>67</v>
@@ -10383,7 +10383,7 @@
         <v>1913</v>
       </c>
       <c r="G432" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H432" t="s">
         <v>67</v>
@@ -10406,7 +10406,7 @@
         <v>1914</v>
       </c>
       <c r="G433" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H433" t="s">
         <v>67</v>
@@ -10429,7 +10429,7 @@
         <v>1915</v>
       </c>
       <c r="G434" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H434" t="s">
         <v>67</v>
@@ -10452,7 +10452,7 @@
         <v>1916</v>
       </c>
       <c r="G435" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H435" t="s">
         <v>67</v>
@@ -10475,7 +10475,7 @@
         <v>1917</v>
       </c>
       <c r="G436" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H436" t="s">
         <v>67</v>
@@ -10498,7 +10498,7 @@
         <v>1918</v>
       </c>
       <c r="G437" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H437" t="s">
         <v>67</v>
@@ -10521,7 +10521,7 @@
         <v>1919</v>
       </c>
       <c r="G438" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H438" t="s">
         <v>67</v>
@@ -10544,7 +10544,7 @@
         <v>1920</v>
       </c>
       <c r="G439" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H439" t="s">
         <v>67</v>
@@ -10567,7 +10567,7 @@
         <v>1921</v>
       </c>
       <c r="G440" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H440" t="s">
         <v>67</v>
@@ -10590,7 +10590,7 @@
         <v>1922</v>
       </c>
       <c r="G441" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H441" t="s">
         <v>67</v>
@@ -10613,7 +10613,7 @@
         <v>1923</v>
       </c>
       <c r="G442" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H442" t="s">
         <v>67</v>
@@ -10636,7 +10636,7 @@
         <v>1924</v>
       </c>
       <c r="G443" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H443" t="s">
         <v>67</v>
@@ -10659,7 +10659,7 @@
         <v>1925</v>
       </c>
       <c r="G444" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H444" t="s">
         <v>67</v>
@@ -10682,7 +10682,7 @@
         <v>1926</v>
       </c>
       <c r="G445" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H445" t="s">
         <v>67</v>
@@ -10705,7 +10705,7 @@
         <v>1927</v>
       </c>
       <c r="G446" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H446" t="s">
         <v>67</v>
@@ -10728,7 +10728,7 @@
         <v>1928</v>
       </c>
       <c r="G447" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H447" t="s">
         <v>67</v>
@@ -10751,7 +10751,7 @@
         <v>1929</v>
       </c>
       <c r="G448" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H448" t="s">
         <v>67</v>
@@ -10774,7 +10774,7 @@
         <v>1930</v>
       </c>
       <c r="G449" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H449" t="s">
         <v>67</v>
@@ -10797,7 +10797,7 @@
         <v>1931</v>
       </c>
       <c r="G450" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H450" t="s">
         <v>67</v>
@@ -10820,7 +10820,7 @@
         <v>1932</v>
       </c>
       <c r="G451" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H451" t="s">
         <v>67</v>
@@ -10843,7 +10843,7 @@
         <v>1933</v>
       </c>
       <c r="G452" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H452" t="s">
         <v>67</v>
@@ -10866,7 +10866,7 @@
         <v>1934</v>
       </c>
       <c r="G453" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H453" t="s">
         <v>67</v>
@@ -10889,7 +10889,7 @@
         <v>1935</v>
       </c>
       <c r="G454" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H454" t="s">
         <v>67</v>
@@ -10912,7 +10912,7 @@
         <v>1936</v>
       </c>
       <c r="G455" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H455" t="s">
         <v>67</v>
@@ -10935,7 +10935,7 @@
         <v>1937</v>
       </c>
       <c r="G456" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H456" t="s">
         <v>67</v>
@@ -10958,7 +10958,7 @@
         <v>1938</v>
       </c>
       <c r="G457" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H457" t="s">
         <v>67</v>
@@ -10981,7 +10981,7 @@
         <v>1939</v>
       </c>
       <c r="G458" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H458" t="s">
         <v>67</v>
@@ -11004,7 +11004,7 @@
         <v>1940</v>
       </c>
       <c r="G459" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H459" t="s">
         <v>67</v>
@@ -11027,7 +11027,7 @@
         <v>1941</v>
       </c>
       <c r="G460" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H460" t="s">
         <v>67</v>
@@ -11050,7 +11050,7 @@
         <v>1945</v>
       </c>
       <c r="G461" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H461" t="s">
         <v>67</v>
@@ -11073,7 +11073,7 @@
         <v>1946</v>
       </c>
       <c r="G462" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H462" t="s">
         <v>67</v>
@@ -11096,7 +11096,7 @@
         <v>1947</v>
       </c>
       <c r="G463" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H463" t="s">
         <v>67</v>
@@ -11119,7 +11119,7 @@
         <v>1948</v>
       </c>
       <c r="G464" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H464" t="s">
         <v>67</v>
@@ -11142,7 +11142,7 @@
         <v>1949</v>
       </c>
       <c r="G465" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H465" t="s">
         <v>67</v>
@@ -11165,7 +11165,7 @@
         <v>1944</v>
       </c>
       <c r="G466" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H466" t="s">
         <v>67</v>
@@ -11188,7 +11188,7 @@
         <v>1957</v>
       </c>
       <c r="G467" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H467" t="s">
         <v>67</v>
@@ -11211,7 +11211,7 @@
         <v>1963</v>
       </c>
       <c r="G468" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H468" t="s">
         <v>67</v>
@@ -11234,7 +11234,7 @@
         <v>1966</v>
       </c>
       <c r="G469" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H469" t="s">
         <v>67</v>

</xml_diff>